<commit_message>
update results into github following Fuentes meeting
</commit_message>
<xml_diff>
--- a/fit_gaussians/results/GMM Plotting.xlsx
+++ b/fit_gaussians/results/GMM Plotting.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="315" windowWidth="17940" windowHeight="7140" activeTab="2"/>
+    <workbookView xWindow="780" yWindow="315" windowWidth="17940" windowHeight="7140" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="GMM Data" sheetId="1" r:id="rId1"/>
@@ -173,13 +173,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -200,17 +200,35 @@
           <a:bodyPr/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr>
-              <a:defRPr/>
+            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Pre</a:t>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0"/>
+              <a:t>Pre Image R vs NR GMM Peaks Intensity (HU)</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Image R vs NR GMM Clusters</a:t>
-            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -218,7 +236,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.12580555555555559"/>
+          <c:x val="0.12580555555555556"/>
           <c:y val="4.1666666666666664E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -313,12 +331,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="98801920"/>
-        <c:axId val="98807808"/>
+        <c:axId val="97366400"/>
+        <c:axId val="97367936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="98801920"/>
+        <c:axId val="97366400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -326,14 +343,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98807808"/>
+        <c:crossAx val="97367936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98807808"/>
+        <c:axId val="97367936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -342,7 +359,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98801920"/>
+        <c:crossAx val="97366400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -355,7 +372,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -375,9 +392,10 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Art Image R vs NR GMM Clusters</a:t>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0"/>
+              <a:t>Art Image R vs NR GMM Peaks Intensity (HU)</a:t>
             </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -385,7 +403,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.12580555555555553"/>
+          <c:x val="0.1258055555555555"/>
           <c:y val="4.1666666666666664E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -459,11 +477,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="185412608"/>
-        <c:axId val="185459456"/>
+        <c:axId val="97484160"/>
+        <c:axId val="97535104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="185412608"/>
+        <c:axId val="97484160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -471,14 +489,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185459456"/>
+        <c:crossAx val="97535104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="185459456"/>
+        <c:axId val="97535104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -487,7 +505,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185412608"/>
+        <c:crossAx val="97484160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -500,7 +518,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -516,13 +534,35 @@
           <a:bodyPr/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr>
-              <a:defRPr/>
+            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Ven Image R vs NR GMM Clusters</a:t>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0"/>
+              <a:t>Ven Image R vs NR GMM Peaks Intensity (HU)</a:t>
             </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -530,7 +570,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.12580555555555548"/>
+          <c:x val="0.12580555555555545"/>
           <c:y val="4.1666666666666664E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -604,11 +644,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="158227840"/>
-        <c:axId val="158258304"/>
+        <c:axId val="113031808"/>
+        <c:axId val="113377664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="158227840"/>
+        <c:axId val="113031808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -616,14 +656,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="158258304"/>
+        <c:crossAx val="113377664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="158258304"/>
+        <c:axId val="113377664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -632,7 +672,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="158227840"/>
+        <c:crossAx val="113031808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -645,7 +685,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -666,7 +706,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Del Image R vs NR GMM Clusters</a:t>
+              <a:t>Del Image R vs NR GMM Peaks Intensity (HU)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -684,6 +724,10 @@
           <c:tx>
             <c:v>Responders</c:v>
           </c:tx>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>Del!$C$3:$C$6</c:f>
@@ -712,6 +756,10 @@
           <c:tx>
             <c:v>Non Responders</c:v>
           </c:tx>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>Del!$D$3:$D$6</c:f>
@@ -734,12 +782,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="180863360"/>
-        <c:axId val="180864896"/>
+        <c:axId val="113411968"/>
+        <c:axId val="113413504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="180863360"/>
+        <c:axId val="113411968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -747,14 +794,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="180864896"/>
+        <c:crossAx val="113413504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="180864896"/>
+        <c:axId val="113413504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -763,7 +810,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="180863360"/>
+        <c:crossAx val="113411968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -776,7 +823,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -786,16 +833,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>28574</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1152525</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>66674</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>266699</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -821,16 +868,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>28574</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1157286</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>90485</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>66674</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>28574</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -856,16 +903,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>28574</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>838200</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:rowOff>42860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>66674</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -891,16 +938,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>42861</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>104774</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
+      <xdr:rowOff>100010</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>80961</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>471487</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6152,7 +6199,7 @@
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="L4" s="7"/>
+      <c r="L4" s="5"/>
     </row>
     <row r="5" spans="1:13">
       <c r="A5">
@@ -6933,7 +6980,7 @@
         <f t="shared" ref="K24:K87" si="8">RANK(G24,$D24:$G24,1)</f>
         <v>4</v>
       </c>
-      <c r="L24" s="7"/>
+      <c r="L24" s="5"/>
     </row>
     <row r="25" spans="1:12">
       <c r="A25">
@@ -7909,7 +7956,7 @@
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="L49" s="7"/>
+      <c r="L49" s="5"/>
     </row>
     <row r="50" spans="1:12">
       <c r="A50">
@@ -9956,8 +10003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26:K35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L3" sqref="L3:N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -9970,10 +10017,10 @@
       <c r="A1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="5"/>
+      <c r="D1" s="7"/>
     </row>
     <row r="2" spans="1:11">
       <c r="C2" s="3" t="s">
@@ -10847,7 +10894,7 @@
   <dimension ref="A1:K71"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:K71"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -10860,10 +10907,10 @@
       <c r="A1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="5"/>
+      <c r="D1" s="7"/>
     </row>
     <row r="2" spans="1:11">
       <c r="C2" s="3" t="s">
@@ -13194,10 +13241,10 @@
       <c r="A1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="5"/>
+      <c r="D1" s="7"/>
     </row>
     <row r="2" spans="1:11">
       <c r="C2" s="3" t="s">
@@ -14070,8 +14117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -14084,10 +14131,10 @@
       <c r="A1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="5"/>
+      <c r="D1" s="7"/>
     </row>
     <row r="2" spans="1:11">
       <c r="C2" s="3" t="s">

</xml_diff>

<commit_message>
update stuff for midterm presentation
</commit_message>
<xml_diff>
--- a/fit_gaussians/results/GMM Plotting.xlsx
+++ b/fit_gaussians/results/GMM Plotting.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="315" windowWidth="17940" windowHeight="7140" activeTab="5"/>
+    <workbookView xWindow="780" yWindow="315" windowWidth="17940" windowHeight="7140" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GMM Data" sheetId="1" r:id="rId1"/>
@@ -226,20 +226,12 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0"/>
-              <a:t>Pre Image R vs NR GMM Peaks Intensity (HU)</a:t>
+              <a:t>Pre, 4-peak GMM Results</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.12580555555555556"/>
-          <c:y val="4.1666666666666664E-2"/>
-        </c:manualLayout>
-      </c:layout>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -331,48 +323,95 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="97366400"/>
-        <c:axId val="97367936"/>
+        <c:axId val="92075520"/>
+        <c:axId val="92077440"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="97366400"/>
+        <c:axId val="92075520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Peak Number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97367936"/>
+        <c:crossAx val="92077440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97367936"/>
+        <c:axId val="92077440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:t>GMM Peak Mean</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                  <a:t> (HU)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1200"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97366400"/>
+        <c:crossAx val="92075520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -403,7 +442,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.1258055555555555"/>
+          <c:x val="0.12580555555555545"/>
           <c:y val="4.1666666666666664E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -477,11 +516,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="97484160"/>
-        <c:axId val="97535104"/>
+        <c:axId val="92418432"/>
+        <c:axId val="92419968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="97484160"/>
+        <c:axId val="92418432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -489,14 +528,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97535104"/>
+        <c:crossAx val="92419968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97535104"/>
+        <c:axId val="92419968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -505,7 +544,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97484160"/>
+        <c:crossAx val="92418432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -518,7 +557,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -560,20 +599,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0"/>
-              <a:t>Ven Image R vs NR GMM Peaks Intensity (HU)</a:t>
+              <a:t>Ven, 4-peak GMM Results</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.12580555555555545"/>
-          <c:y val="4.1666666666666664E-2"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -590,6 +622,27 @@
             <c:errBarType val="both"/>
             <c:errValType val="stdErr"/>
           </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>Pre!$B$3:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Ven!$C$3:$C$6</c:f>
@@ -644,35 +697,75 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="113031808"/>
-        <c:axId val="113377664"/>
+        <c:axId val="80614144"/>
+        <c:axId val="80616064"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="113031808"/>
+        <c:axId val="80614144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Peak Number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113377664"/>
+        <c:crossAx val="80616064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113377664"/>
+        <c:axId val="80616064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:t>GMM Peak Mean</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                  <a:t> (HU)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1200"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113031808"/>
+        <c:crossAx val="80614144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -680,12 +773,22 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -711,7 +814,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -782,11 +884,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="113411968"/>
-        <c:axId val="113413504"/>
+        <c:axId val="91667840"/>
+        <c:axId val="91894912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="113411968"/>
+        <c:axId val="91667840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -794,14 +896,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113413504"/>
+        <c:crossAx val="91894912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113413504"/>
+        <c:axId val="91894912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -810,20 +912,19 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113411968"/>
+        <c:crossAx val="91667840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -833,16 +934,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1152525</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>114299</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>4761</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>266699</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>490536</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -868,16 +969,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1157286</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>90485</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>142873</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>76198</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>28574</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>276224</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -903,20 +1004,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>838200</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>42860</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>357187</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -10004,7 +10105,7 @@
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L3" sqref="L3:N7"/>
+      <selection activeCell="Y23" sqref="Y23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -10893,8 +10994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K71"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -13227,8 +13328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:K35"/>
+    <sheetView tabSelected="1" topLeftCell="G10" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -14117,7 +14218,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>

</xml_diff>